<commit_message>
Added comparison of serial vs parallel map
</commit_message>
<xml_diff>
--- a/spikes/3.1.3/comparison/pjs_map_seq_vs_par_jsperf.xlsx
+++ b/spikes/3.1.3/comparison/pjs_map_seq_vs_par_jsperf.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15700" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28780" windowHeight="15700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -280,21 +280,47 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2136215944"/>
-        <c:axId val="-2137927656"/>
+        <c:axId val="2076156920"/>
+        <c:axId val="2074908232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2136215944"/>
+        <c:axId val="2076156920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:t>#</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                  <a:t> of elements (log scale)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2137927656"/>
+        <c:crossAx val="2074908232"/>
         <c:crossesAt val="1.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -302,18 +328,50 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2137927656"/>
+        <c:axId val="2074908232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:t>Relative</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                  <a:t> p</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:t>erformance</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                  <a:t> of parallel compared to serial</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2136215944"/>
+        <c:crossAx val="2076156920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -322,6 +380,16 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -340,15 +408,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -725,7 +793,7 @@
   <dimension ref="B1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+      <selection activeCell="R34" sqref="R34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Finished first paper draft
</commit_message>
<xml_diff>
--- a/spikes/3.1.3/comparison/pjs_map_seq_vs_par_jsperf.xlsx
+++ b/spikes/3.1.3/comparison/pjs_map_seq_vs_par_jsperf.xlsx
@@ -658,8 +658,24 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="plus"/>
+            <c:size val="12"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -876,10 +892,10 @@
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>177800</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>181786</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1506,7 +1522,7 @@
   <dimension ref="B1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Updated major comparison to firefox 41 nightly
</commit_message>
<xml_diff>
--- a/spikes/3.1.3/comparison/pjs_map_seq_vs_par_jsperf.xlsx
+++ b/spikes/3.1.3/comparison/pjs_map_seq_vs_par_jsperf.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15720" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3200" yWindow="0" windowWidth="25600" windowHeight="15720" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ArrayBuffer" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Amount</t>
   </si>
@@ -52,7 +52,10 @@
     <t>Parallel</t>
   </si>
   <si>
-    <t>Firefox 40</t>
+    <t>Firefox 41</t>
+  </si>
+  <si>
+    <t>Column1</t>
   </si>
 </sst>
 </file>
@@ -162,13 +165,13 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -190,7 +193,7 @@
   <dxfs count="7">
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -199,17 +202,12 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
     <dxf>
       <font>
@@ -222,11 +220,12 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="13"/>
         <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
       </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
     <dxf>
       <font>
@@ -303,16 +302,15 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="13"/>
+        <sz val="12"/>
         <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -321,12 +319,17 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -497,11 +500,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2093655976"/>
-        <c:axId val="2093661736"/>
+        <c:axId val="2109431944"/>
+        <c:axId val="2109439080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2093655976"/>
+        <c:axId val="2109431944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -530,14 +533,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2093661736"/>
+        <c:crossAx val="2109439080"/>
         <c:crossesAt val="1.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -545,7 +547,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2093661736"/>
+        <c:axId val="2109439080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -581,21 +583,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2093655976"/>
+        <c:crossAx val="2109431944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -653,7 +653,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Firefox 40</c:v>
+                  <c:v>Firefox 41</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -703,24 +703,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Table6[Firefox 40]</c:f>
+              <c:f>SharedArrayBuffer!$C$12:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.00244234081402727</c:v>
+                  <c:v>0.00230623738776429</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0210994146687896</c:v>
+                  <c:v>0.0217525660756917</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.175958385163406</c:v>
+                  <c:v>0.191115334362751</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.983258928571429</c:v>
+                  <c:v>1.087264150943396</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.952941176470588</c:v>
+                  <c:v>2.036012401621751</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -737,11 +737,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2097813672"/>
-        <c:axId val="2097837816"/>
+        <c:axId val="2108017880"/>
+        <c:axId val="2062494728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2097813672"/>
+        <c:axId val="2108017880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -770,7 +770,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097837816"/>
+        <c:crossAx val="2062494728"/>
         <c:crossesAt val="1.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -778,7 +778,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2097837816"/>
+        <c:axId val="2062494728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -814,7 +814,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097813672"/>
+        <c:crossAx val="2108017880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.4"/>
@@ -948,23 +948,24 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table25" displayName="Table25" ref="B1:D6" totalsRowShown="0">
-  <autoFilter ref="B1:D6"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table25" displayName="Table25" ref="B1:E6" totalsRowShown="0">
+  <autoFilter ref="B1:E6"/>
+  <tableColumns count="4">
     <tableColumn id="1" name="Elements"/>
-    <tableColumn id="2" name="Seq" dataDxfId="5"/>
-    <tableColumn id="3" name="Parallel" dataDxfId="6"/>
+    <tableColumn id="2" name="Seq" dataDxfId="1"/>
+    <tableColumn id="3" name="Parallel" dataDxfId="0"/>
+    <tableColumn id="4" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B11:C16" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" tableBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B11:C16" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
   <autoFilter ref="B11:C16"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Elements" dataDxfId="3"/>
-    <tableColumn id="2" name="Firefox 40" dataDxfId="2">
+    <tableColumn id="2" name="Firefox 41" dataDxfId="2">
       <calculatedColumnFormula>D2/C2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1310,14 +1311,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6">
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="5"/>
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" spans="2:6">
       <c r="B2" t="s">
@@ -1519,10 +1520,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D16"/>
+  <dimension ref="B1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1532,7 +1533,7 @@
     <col min="4" max="4" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4">
+    <row r="1" spans="2:5">
       <c r="B1" t="s">
         <v>7</v>
       </c>
@@ -1542,113 +1543,119 @@
       <c r="D1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="2:4" ht="16">
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" ht="16">
       <c r="B2">
         <v>2</v>
       </c>
-      <c r="C2" s="4">
-        <v>154442</v>
-      </c>
-      <c r="D2" s="4">
-        <v>377.2</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" ht="16">
+      <c r="C2" s="3">
+        <v>142223</v>
+      </c>
+      <c r="D2" s="3">
+        <v>328</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="16">
       <c r="B3">
         <v>3</v>
       </c>
-      <c r="C3" s="4">
-        <v>17460.2</v>
-      </c>
-      <c r="D3" s="4">
-        <v>368.4</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" ht="16">
+      <c r="C3" s="3">
+        <v>16503.8</v>
+      </c>
+      <c r="D3" s="3">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="16">
       <c r="B4">
         <v>4</v>
       </c>
-      <c r="C4" s="4">
-        <v>1768.6</v>
-      </c>
-      <c r="D4" s="4">
-        <v>311.2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" ht="16">
+      <c r="C4" s="3">
+        <v>1683.8</v>
+      </c>
+      <c r="D4" s="3">
+        <v>321.8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="16">
       <c r="B5">
         <v>5</v>
       </c>
-      <c r="C5" s="4">
-        <v>179.2</v>
-      </c>
-      <c r="D5" s="4">
-        <v>176.2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" ht="16">
+      <c r="C5" s="3">
+        <v>169.6</v>
+      </c>
+      <c r="D5" s="3">
+        <v>184.4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="16">
       <c r="B6">
         <v>6</v>
       </c>
-      <c r="C6" s="4">
-        <v>17</v>
-      </c>
-      <c r="D6" s="4">
-        <v>33.200000000000003</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4">
-      <c r="B11" s="5" t="s">
+      <c r="C6" s="3">
+        <v>16.771999999999998</v>
+      </c>
+      <c r="D6" s="3">
+        <v>34.148000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="2:4">
-      <c r="B12" s="2">
+    <row r="12" spans="2:5">
+      <c r="B12" s="1">
         <v>2</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <f>D2/C2</f>
-        <v>2.4423408140272721E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4">
-      <c r="B13" s="2">
+        <v>2.3062373877642856E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="B13" s="1">
         <v>3</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <f t="shared" ref="C13:C16" si="0">D3/C3</f>
-        <v>2.1099414668789587E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4">
-      <c r="B14" s="2">
+        <v>2.1752566075691659E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="B14" s="1">
         <v>4</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <f t="shared" si="0"/>
-        <v>0.17595838516340609</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4">
-      <c r="B15" s="2">
+        <v>0.19111533436275094</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5">
+      <c r="B15" s="1">
         <v>5</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <f t="shared" si="0"/>
-        <v>0.9832589285714286</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4">
-      <c r="B16" s="3">
+        <v>1.0872641509433962</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5">
+      <c r="B16" s="2">
         <v>6</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <f t="shared" si="0"/>
-        <v>1.9529411764705884</v>
+        <v>2.0360124016217509</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated chart comparing linerar vs parallel
</commit_message>
<xml_diff>
--- a/spikes/3.1.3/comparison/pjs_map_seq_vs_par_jsperf.xlsx
+++ b/spikes/3.1.3/comparison/pjs_map_seq_vs_par_jsperf.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="0" windowWidth="25600" windowHeight="15720" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ArrayBuffer" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>Amount</t>
   </si>
@@ -56,6 +56,15 @@
   </si>
   <si>
     <t>Column1</t>
+  </si>
+  <si>
+    <t>Firefox 41 Nightly</t>
+  </si>
+  <si>
+    <t>Par ops (FF)</t>
+  </si>
+  <si>
+    <t>Seq ops (FF)</t>
   </si>
 </sst>
 </file>
@@ -146,7 +155,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -162,8 +171,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -172,8 +185,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -181,6 +195,8 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -188,9 +204,17 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="9">
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -404,19 +428,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0105750237965546</c:v>
+                  <c:v>0.00808261497012231</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0917371175523349</c:v>
+                  <c:v>0.0736953990990535</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.522627737226277</c:v>
+                  <c:v>0.436274509803922</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.144927536231884</c:v>
+                  <c:v>1.024038461538461</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.421052631578947</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -471,19 +495,86 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0105388349720022</c:v>
+                  <c:v>0.00950659645951979</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0873449692765861</c:v>
+                  <c:v>0.0769351793580868</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.554491017964072</c:v>
+                  <c:v>0.46029919447641</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.003597122302158</c:v>
+                  <c:v>1.037878787878788</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1.24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ArrayBuffer!$E$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Firefox 41</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ArrayBuffer!$B$11:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ArrayBuffer!$E$11:$E$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.0111356186625004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.09736680955297</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.511912865895167</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.099337748344371</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.428571428571429</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -500,11 +591,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2109431944"/>
-        <c:axId val="2109439080"/>
+        <c:axId val="2117571912"/>
+        <c:axId val="2117577672"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2109431944"/>
+        <c:axId val="2117571912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -533,13 +624,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109439080"/>
+        <c:crossAx val="2117577672"/>
         <c:crossesAt val="1.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -547,7 +639,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2109439080"/>
+        <c:axId val="2117577672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -583,19 +675,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109431944"/>
+        <c:crossAx val="2117571912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -708,19 +802,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.00230623738776429</c:v>
+                  <c:v>0.00294856477652176</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0217525660756917</c:v>
+                  <c:v>0.0286453017622644</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.191115334362751</c:v>
+                  <c:v>0.243022464261402</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.087264150943396</c:v>
+                  <c:v>1.245033112582781</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.036012401621751</c:v>
+                  <c:v>2.285714285714286</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -737,11 +831,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2108017880"/>
-        <c:axId val="2062494728"/>
+        <c:axId val="2116992328"/>
+        <c:axId val="2117002456"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2108017880"/>
+        <c:axId val="2116992328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -770,7 +864,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2062494728"/>
+        <c:crossAx val="2117002456"/>
         <c:crossesAt val="1.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -778,7 +872,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2062494728"/>
+        <c:axId val="2117002456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -814,7 +908,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2108017880"/>
+        <c:crossAx val="2116992328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.4"/>
@@ -851,16 +945,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>447488</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -918,29 +1012,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:F7" totalsRowShown="0">
-  <autoFilter ref="B2:F7"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:H7" totalsRowShown="0">
+  <autoFilter ref="B2:H7"/>
+  <tableColumns count="7">
     <tableColumn id="1" name="Amount"/>
     <tableColumn id="2" name="Par ops (40)"/>
     <tableColumn id="3" name="Seq ops (40)"/>
     <tableColumn id="4" name="Par ops (41)"/>
     <tableColumn id="5" name="Seq (41)"/>
+    <tableColumn id="6" name="Par ops (FF)"/>
+    <tableColumn id="7" name="Seq ops (FF)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:D15" totalsRowShown="0">
-  <autoFilter ref="B10:D15"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:E15" totalsRowShown="0">
+  <autoFilter ref="B10:E15"/>
+  <tableColumns count="4">
     <tableColumn id="1" name="Elements"/>
     <tableColumn id="2" name="Chrome 40">
       <calculatedColumnFormula>C3/D3</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="Chrome 41">
       <calculatedColumnFormula>E3/F3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="Firefox 41" dataDxfId="1">
+      <calculatedColumnFormula>G3/H3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -952,8 +1051,8 @@
   <autoFilter ref="B1:E6"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Elements"/>
-    <tableColumn id="2" name="Seq" dataDxfId="1"/>
-    <tableColumn id="3" name="Parallel" dataDxfId="0"/>
+    <tableColumn id="2" name="Seq" dataDxfId="3"/>
+    <tableColumn id="3" name="Parallel" dataDxfId="2"/>
     <tableColumn id="4" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -961,11 +1060,11 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B11:C16" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B11:C16" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
   <autoFilter ref="B11:C16"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Elements" dataDxfId="3"/>
-    <tableColumn id="2" name="Firefox 41" dataDxfId="2">
+    <tableColumn id="1" name="Elements" dataDxfId="5"/>
+    <tableColumn id="2" name="Firefox 41" dataDxfId="4">
       <calculatedColumnFormula>D2/C2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1295,10 +1394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F15"/>
+  <dimension ref="B1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1308,9 +1407,11 @@
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" customWidth="1"/>
+    <col min="8" max="8" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6">
+    <row r="1" spans="2:8">
       <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
@@ -1319,8 +1420,12 @@
         <v>2</v>
       </c>
       <c r="F1" s="5"/>
-    </row>
-    <row r="2" spans="2:6">
+      <c r="G1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="5"/>
+    </row>
+    <row r="2" spans="2:8">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -1336,84 +1441,114 @@
       <c r="F2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="2:6">
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8">
       <c r="B3">
         <v>100</v>
       </c>
       <c r="C3">
-        <v>1922</v>
+        <v>1473</v>
       </c>
       <c r="D3">
-        <v>181749</v>
+        <v>182243</v>
       </c>
       <c r="E3">
-        <v>2490</v>
+        <v>2125</v>
       </c>
       <c r="F3">
-        <v>236269</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6">
+        <v>223529</v>
+      </c>
+      <c r="G3">
+        <v>1454</v>
+      </c>
+      <c r="H3" s="6">
+        <v>130572</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8">
       <c r="B4">
         <v>1000</v>
       </c>
       <c r="C4">
-        <v>1823</v>
+        <v>1456</v>
       </c>
       <c r="D4">
-        <v>19872</v>
+        <v>19757</v>
       </c>
       <c r="E4">
-        <v>2317</v>
+        <v>1956</v>
       </c>
       <c r="F4">
-        <v>26527</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6">
+        <v>25424</v>
+      </c>
+      <c r="G4">
+        <v>1431</v>
+      </c>
+      <c r="H4" s="6">
+        <v>14697</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8">
       <c r="B5">
         <v>10000</v>
       </c>
       <c r="C5">
-        <v>1074</v>
+        <v>890</v>
       </c>
       <c r="D5">
-        <v>2055</v>
+        <v>2040</v>
       </c>
       <c r="E5">
-        <v>1389</v>
+        <v>1200</v>
       </c>
       <c r="F5">
-        <v>2505</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6">
+        <v>2607</v>
+      </c>
+      <c r="G5">
+        <v>752</v>
+      </c>
+      <c r="H5" s="6">
+        <v>1469</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8">
       <c r="B6">
         <v>100000</v>
       </c>
       <c r="C6">
-        <v>237</v>
+        <v>213</v>
       </c>
       <c r="D6">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E6">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="F6">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6">
+        <v>264</v>
+      </c>
+      <c r="G6">
+        <v>166</v>
+      </c>
+      <c r="H6">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8">
       <c r="B7">
         <v>1000000</v>
       </c>
       <c r="C7">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D7">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E7">
         <v>31</v>
@@ -1421,8 +1556,14 @@
       <c r="F7">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="2:6">
+      <c r="G7">
+        <v>20</v>
+      </c>
+      <c r="H7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -1432,76 +1573,100 @@
       <c r="D10" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="2:6">
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8">
       <c r="B11">
         <v>2</v>
       </c>
       <c r="C11">
         <f>C3/D3</f>
-        <v>1.0575023796554589E-2</v>
+        <v>8.082614970122309E-3</v>
       </c>
       <c r="D11">
         <f>E3/F3</f>
-        <v>1.0538834972002252E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6">
+        <v>9.5065964595197946E-3</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ref="E11:E15" si="0">G3/H3</f>
+        <v>1.1135618662500383E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8">
       <c r="B12">
         <v>3</v>
       </c>
       <c r="C12">
-        <f t="shared" ref="C12:C15" si="0">C4/D4</f>
-        <v>9.1737117552334949E-2</v>
+        <f t="shared" ref="C12:C15" si="1">C4/D4</f>
+        <v>7.3695399099053496E-2</v>
       </c>
       <c r="D12">
-        <f t="shared" ref="D12:D15" si="1">E4/F4</f>
-        <v>8.7344969276586124E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6">
+        <f t="shared" ref="D12:D15" si="2">E4/F4</f>
+        <v>7.6935179358086844E-2</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>9.7366809552969988E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8">
       <c r="B13">
         <v>4</v>
       </c>
       <c r="C13">
+        <f t="shared" si="1"/>
+        <v>0.43627450980392157</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>0.46029919447640966</v>
+      </c>
+      <c r="E13">
         <f t="shared" si="0"/>
-        <v>0.52262773722627742</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="1"/>
-        <v>0.55449101796407185</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6">
+        <v>0.51191286589516682</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8">
       <c r="B14">
         <v>5</v>
       </c>
       <c r="C14">
+        <f t="shared" si="1"/>
+        <v>1.0240384615384615</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="2"/>
+        <v>1.0378787878787878</v>
+      </c>
+      <c r="E14">
         <f t="shared" si="0"/>
-        <v>1.144927536231884</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="1"/>
-        <v>1.0035971223021583</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6">
+        <v>1.0993377483443709</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8">
       <c r="B15">
         <v>6</v>
       </c>
       <c r="C15">
+        <f t="shared" si="1"/>
+        <v>1.2</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>1.24</v>
+      </c>
+      <c r="E15">
         <f t="shared" si="0"/>
-        <v>1.4210526315789473</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="1"/>
-        <v>1.24</v>
+        <v>1.4285714285714286</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1522,8 +1687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1552,10 +1717,10 @@
         <v>2</v>
       </c>
       <c r="C2" s="3">
-        <v>142223</v>
+        <v>130572</v>
       </c>
       <c r="D2" s="3">
-        <v>328</v>
+        <v>385</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1566,10 +1731,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="3">
-        <v>16503.8</v>
+        <v>14697</v>
       </c>
       <c r="D3" s="3">
-        <v>359</v>
+        <v>421</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="16">
@@ -1577,10 +1742,10 @@
         <v>4</v>
       </c>
       <c r="C4" s="3">
-        <v>1683.8</v>
+        <v>1469</v>
       </c>
       <c r="D4" s="3">
-        <v>321.8</v>
+        <v>357</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="16">
@@ -1588,10 +1753,10 @@
         <v>5</v>
       </c>
       <c r="C5" s="3">
-        <v>169.6</v>
+        <v>151</v>
       </c>
       <c r="D5" s="3">
-        <v>184.4</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="16">
@@ -1599,10 +1764,10 @@
         <v>6</v>
       </c>
       <c r="C6" s="3">
-        <v>16.771999999999998</v>
+        <v>14</v>
       </c>
       <c r="D6" s="3">
-        <v>34.148000000000003</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="2:5">
@@ -1619,7 +1784,7 @@
       </c>
       <c r="C12" s="1">
         <f>D2/C2</f>
-        <v>2.3062373877642856E-3</v>
+        <v>2.9485647765217656E-3</v>
       </c>
     </row>
     <row r="13" spans="2:5">
@@ -1628,7 +1793,7 @@
       </c>
       <c r="C13" s="1">
         <f t="shared" ref="C13:C16" si="0">D3/C3</f>
-        <v>2.1752566075691659E-2</v>
+        <v>2.8645301762264409E-2</v>
       </c>
     </row>
     <row r="14" spans="2:5">
@@ -1637,7 +1802,7 @@
       </c>
       <c r="C14" s="1">
         <f t="shared" si="0"/>
-        <v>0.19111533436275094</v>
+        <v>0.24302246426140231</v>
       </c>
     </row>
     <row r="15" spans="2:5">
@@ -1646,7 +1811,7 @@
       </c>
       <c r="C15" s="1">
         <f t="shared" si="0"/>
-        <v>1.0872641509433962</v>
+        <v>1.2450331125827814</v>
       </c>
     </row>
     <row r="16" spans="2:5">
@@ -1655,7 +1820,7 @@
       </c>
       <c r="C16" s="1">
         <f t="shared" si="0"/>
-        <v>2.0360124016217509</v>
+        <v>2.2857142857142856</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixes for map serial vs parallel cmp
</commit_message>
<xml_diff>
--- a/spikes/3.1.3/comparison/pjs_map_seq_vs_par_jsperf.xlsx
+++ b/spikes/3.1.3/comparison/pjs_map_seq_vs_par_jsperf.xlsx
@@ -182,10 +182,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -209,48 +209,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -355,6 +313,48 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
@@ -591,11 +591,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2117571912"/>
-        <c:axId val="2117577672"/>
+        <c:axId val="2084363880"/>
+        <c:axId val="2084371016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2117571912"/>
+        <c:axId val="2084363880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -610,17 +610,17 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200"/>
+                  <a:defRPr sz="1400"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:rPr lang="en-US" sz="1400"/>
                   <a:t>#</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
                   <a:t> of elements (log scale)</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US" sz="1200"/>
+                <a:endParaRPr lang="en-US" sz="1400"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -631,7 +631,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117577672"/>
+        <c:crossAx val="2084371016"/>
         <c:crossesAt val="1.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -639,7 +639,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2117577672"/>
+        <c:axId val="2084371016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -653,25 +653,25 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200"/>
+                  <a:defRPr sz="1400"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:rPr lang="en-US" sz="1400"/>
                   <a:t>Relative</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
                   <a:t> p</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:rPr lang="en-US" sz="1400"/>
                   <a:t>erformance</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
                   <a:t> of parallel compared to serial</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US" sz="1200"/>
+                <a:endParaRPr lang="en-US" sz="1400"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -682,7 +682,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117571912"/>
+        <c:crossAx val="2084363880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -696,7 +696,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200"/>
+            <a:defRPr sz="1400"/>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
         </a:p>
@@ -729,7 +729,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -831,11 +830,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2116992328"/>
-        <c:axId val="2117002456"/>
+        <c:axId val="2082454104"/>
+        <c:axId val="2081794712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2116992328"/>
+        <c:axId val="2082454104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -857,14 +856,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117002456"/>
+        <c:crossAx val="2081794712"/>
         <c:crossesAt val="1.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -872,7 +870,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2117002456"/>
+        <c:axId val="2081794712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -901,14 +899,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116992328"/>
+        <c:crossAx val="2082454104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.4"/>
@@ -916,7 +913,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1021,7 +1017,7 @@
     <tableColumn id="4" name="Par ops (41)"/>
     <tableColumn id="5" name="Seq (41)"/>
     <tableColumn id="6" name="Par ops (FF)"/>
-    <tableColumn id="7" name="Seq ops (FF)" dataDxfId="0"/>
+    <tableColumn id="7" name="Seq ops (FF)" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1038,7 +1034,7 @@
     <tableColumn id="3" name="Chrome 41">
       <calculatedColumnFormula>E3/F3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Firefox 41" dataDxfId="1">
+    <tableColumn id="4" name="Firefox 41" dataDxfId="7">
       <calculatedColumnFormula>G3/H3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1051,8 +1047,8 @@
   <autoFilter ref="B1:E6"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Elements"/>
-    <tableColumn id="2" name="Seq" dataDxfId="3"/>
-    <tableColumn id="3" name="Parallel" dataDxfId="2"/>
+    <tableColumn id="2" name="Seq" dataDxfId="6"/>
+    <tableColumn id="3" name="Parallel" dataDxfId="5"/>
     <tableColumn id="4" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1060,11 +1056,11 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B11:C16" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B11:C16" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3" tableBorderDxfId="2">
   <autoFilter ref="B11:C16"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Elements" dataDxfId="5"/>
-    <tableColumn id="2" name="Firefox 41" dataDxfId="4">
+    <tableColumn id="1" name="Elements" dataDxfId="1"/>
+    <tableColumn id="2" name="Firefox 41" dataDxfId="0">
       <calculatedColumnFormula>D2/C2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1396,8 +1392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
+      <selection activeCell="T29" sqref="T29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1412,18 +1408,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8">
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5" t="s">
+      <c r="D1" s="6"/>
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5" t="s">
+      <c r="F1" s="6"/>
+      <c r="G1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="5"/>
+      <c r="H1" s="6"/>
     </row>
     <row r="2" spans="2:8">
       <c r="B2" t="s">
@@ -1467,7 +1463,7 @@
       <c r="G3">
         <v>1454</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5">
         <v>130572</v>
       </c>
     </row>
@@ -1490,7 +1486,7 @@
       <c r="G4">
         <v>1431</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <v>14697</v>
       </c>
     </row>
@@ -1513,7 +1509,7 @@
       <c r="G5">
         <v>752</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <v>1469</v>
       </c>
     </row>

</xml_diff>